<commit_message>
Support const char * argument type and size_t return type.
</commit_message>
<xml_diff>
--- a/XllExamples/Examples.xlsx
+++ b/XllExamples/Examples.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>Arithmetic Example</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -83,6 +83,18 @@
   </si>
   <si>
     <t>cba</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MultiByteStrLen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hello</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -428,9 +440,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H18"/>
+  <dimension ref="B2:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
@@ -578,83 +592,128 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B14" s="1" t="s">
-        <v>9</v>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2">
+        <f ca="1">_xll.MultiByteStrLen(C12)</f>
+        <v>5</v>
+      </c>
+      <c r="G12" s="2">
+        <v>5</v>
+      </c>
+      <c r="H12" s="2" t="b">
+        <f ca="1">F12=G12</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="2">
+        <v>256</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2" t="e">
+        <f>_xll.MultiByteStrLen(REPT(C13,D13))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G13" s="2">
+        <f>LEN(C13)*D13</f>
+        <v>256</v>
+      </c>
+      <c r="H13" s="2" t="e">
+        <f>F13=G13</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="2">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
         <v>2</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E17" s="2">
         <v>3</v>
       </c>
-      <c r="F16" s="2">
-        <f ca="1">_xll.Trace(C16:E18)</f>
+      <c r="F17" s="2">
+        <f ca="1">_xll.Trace(C17:E19)</f>
         <v>15</v>
       </c>
-      <c r="G16" s="2">
-        <f>C16+D17+E18</f>
+      <c r="G17" s="2">
+        <f>C17+D18+E19</f>
         <v>15</v>
       </c>
-      <c r="H16" s="2" t="b">
-        <f ca="1">F16=G16</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.15">
-      <c r="C17" s="2">
+      <c r="H17" s="2" t="b">
+        <f ca="1">F17=G17</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="C18" s="2">
         <v>4</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D18" s="2">
         <v>5</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E18" s="2">
         <v>6</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.15">
-      <c r="C18" s="2">
-        <v>7</v>
-      </c>
-      <c r="D18" s="2">
-        <v>8</v>
-      </c>
-      <c r="E18" s="2">
-        <v>9</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="C19" s="2">
+        <v>7</v>
+      </c>
+      <c r="D19" s="2">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2">
+        <v>9</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Rename ArgumentWrapper to ArgumentMarshaler.
</commit_message>
<xml_diff>
--- a/XllExamples/Examples.xlsx
+++ b/XllExamples/Examples.xlsx
@@ -443,7 +443,7 @@
   <dimension ref="B2:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -621,20 +621,20 @@
         <v>17</v>
       </c>
       <c r="D13" s="2">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="2" t="e">
-        <f>_xll.MultiByteStrLen(REPT(C13,D13))</f>
-        <v>#VALUE!</v>
+      <c r="F13" s="2">
+        <f ca="1">_xll.MultiByteStrLen(REPT(C13,D13))</f>
+        <v>255</v>
       </c>
       <c r="G13" s="2">
         <f>LEN(C13)*D13</f>
-        <v>256</v>
-      </c>
-      <c r="H13" s="2" t="e">
-        <f>F13=G13</f>
-        <v>#VALUE!</v>
+        <v>255</v>
+      </c>
+      <c r="H13" s="2" t="b">
+        <f ca="1">F13=G13</f>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Add support to marshal VARIANT.
</commit_message>
<xml_diff>
--- a/XllExamples/Examples.xlsx
+++ b/XllExamples/Examples.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>Arithmetic Example</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -95,6 +95,30 @@
   </si>
   <si>
     <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Variant Example</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VariantType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hello</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>double</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -102,6 +126,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="177" formatCode="yyyy/mm/dd"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -147,7 +174,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -159,6 +186,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -440,17 +470,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H19"/>
+  <dimension ref="B2:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
+    <col min="3" max="3" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.15">
@@ -547,48 +576,69 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="str">
+        <f>_xll.ReverseString(C10)</f>
+        <v>cba</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="H10" s="2" t="b">
+        <f>F10=G10</f>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2" t="str">
-        <f>_xll.ReverseString(C11)</f>
-        <v>cba</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>14</v>
+      <c r="F11" s="2">
+        <f ca="1">_xll.MultiByteStrLen(C11)</f>
+        <v>5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>5</v>
       </c>
       <c r="H11" s="2" t="b">
-        <f>F11=G11</f>
+        <f ca="1">F11=G11</f>
         <v>1</v>
       </c>
     </row>
@@ -597,123 +647,187 @@
         <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="D12" s="2">
+        <v>255</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2">
-        <f ca="1">_xll.MultiByteStrLen(C12)</f>
-        <v>5</v>
+        <f ca="1">_xll.MultiByteStrLen(REPT(C12,D12))</f>
+        <v>255</v>
       </c>
       <c r="G12" s="2">
-        <v>5</v>
+        <f>LEN(C12)*D12</f>
+        <v>255</v>
       </c>
       <c r="H12" s="2" t="b">
         <f ca="1">F12=G12</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="2">
-        <v>255</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2">
-        <f ca="1">_xll.MultiByteStrLen(REPT(C13,D13))</f>
-        <v>255</v>
-      </c>
-      <c r="G13" s="2">
-        <f>LEN(C13)*D13</f>
-        <v>255</v>
-      </c>
-      <c r="H13" s="2" t="b">
-        <f ca="1">F13=G13</f>
-        <v>1</v>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B14" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
         <v>2</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="E16" s="2">
         <v>3</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="2">
+        <f ca="1">_xll.Trace(C16:E18)</f>
+        <v>15</v>
+      </c>
+      <c r="G16" s="2">
+        <f>C16+D17+E18</f>
+        <v>15</v>
+      </c>
+      <c r="H16" s="2" t="b">
+        <f ca="1">F16=G16</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="C17" s="2">
         <v>4</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="D17" s="2">
         <v>5</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="E17" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="2">
-        <v>1</v>
-      </c>
-      <c r="D17" s="2">
-        <v>2</v>
-      </c>
-      <c r="E17" s="2">
-        <v>3</v>
-      </c>
-      <c r="F17" s="2">
-        <f ca="1">_xll.Trace(C17:E19)</f>
-        <v>15</v>
-      </c>
-      <c r="G17" s="2">
-        <f>C17+D18+E19</f>
-        <v>15</v>
-      </c>
-      <c r="H17" s="2" t="b">
-        <f ca="1">F17=G17</f>
-        <v>1</v>
-      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.15">
       <c r="C18" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D18" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E18" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="C19" s="2">
-        <v>7</v>
-      </c>
-      <c r="D19" s="2">
-        <v>8</v>
-      </c>
-      <c r="E19" s="2">
-        <v>9</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2" t="str">
+        <f ca="1">_xll.VariantType(C22)</f>
+        <v>string</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="2" t="b">
+        <f ca="1">F22=G22</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="2">
+        <v>100</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2" t="str">
+        <f ca="1">_xll.VariantType(C23)</f>
+        <v>double</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" s="2" t="b">
+        <f ca="1">F23=G23</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="4">
+        <v>40179</v>
+      </c>
+      <c r="F24" s="2" t="str">
+        <f ca="1">_xll.VariantType(C24)</f>
+        <v>double</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" s="2" t="b">
+        <f ca="1">F24=G24</f>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Marshal Ansi string as Unicode string.
</commit_message>
<xml_diff>
--- a/XllExamples/Examples.xlsx
+++ b/XllExamples/Examples.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
   <si>
     <t>Arithmetic Example</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,10 +87,6 @@
   </si>
   <si>
     <t>MultiByteStrLen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hello</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -127,7 +123,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -187,7 +183,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -472,7 +468,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
@@ -628,14 +626,17 @@
       <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2">
+        <v>255</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2">
-        <f ca="1">_xll.MultiByteStrLen(C11)</f>
-        <v>5</v>
+        <f ca="1">_xll.MultiByteStrLen(REPT(C11,D11))</f>
+        <v>255</v>
       </c>
       <c r="G11" s="2">
-        <v>5</v>
+        <f>LEN(C11)*D11</f>
+        <v>255</v>
       </c>
       <c r="H11" s="2" t="b">
         <f ca="1">F11=G11</f>
@@ -647,19 +648,19 @@
         <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="2">
-        <v>255</v>
+        <v>500</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2">
         <f ca="1">_xll.MultiByteStrLen(REPT(C12,D12))</f>
-        <v>255</v>
+        <v>500</v>
       </c>
       <c r="G12" s="2">
         <f>LEN(C12)*D12</f>
-        <v>255</v>
+        <v>500</v>
       </c>
       <c r="H12" s="2" t="b">
         <f ca="1">F12=G12</f>
@@ -746,12 +747,12 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>3</v>
@@ -770,10 +771,10 @@
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -782,7 +783,7 @@
         <v>string</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H22" s="2" t="b">
         <f ca="1">F22=G22</f>
@@ -791,7 +792,7 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="2">
         <v>100</v>
@@ -803,7 +804,7 @@
         <v>double</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H23" s="2" t="b">
         <f ca="1">F23=G23</f>
@@ -812,7 +813,7 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B24" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24" s="4">
         <v>40179</v>
@@ -822,7 +823,7 @@
         <v>double</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H24" s="2" t="b">
         <f ca="1">F24=G24</f>

</xml_diff>

<commit_message>
Move type text related functions into TypeText.h.
</commit_message>
<xml_diff>
--- a/XllExamples/Examples.xlsx
+++ b/XllExamples/Examples.xlsx
@@ -170,7 +170,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -185,6 +185,9 @@
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,15 +472,15 @@
   <dimension ref="B2:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="1"/>
+    <col min="3" max="4" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.15">
@@ -818,8 +821,12 @@
       <c r="C24" s="4">
         <v>40179</v>
       </c>
+      <c r="D24" s="5">
+        <f>C24</f>
+        <v>40179</v>
+      </c>
       <c r="F24" s="2" t="str">
-        <f ca="1">_xll.VariantType(C24)</f>
+        <f ca="1">_xll.VariantType(C24,D24)</f>
         <v>double</v>
       </c>
       <c r="G24" s="2" t="s">

</xml_diff>

<commit_message>
Support exporting udf in custom namespace with renaming.
</commit_message>
<xml_diff>
--- a/XllExamples/Examples.xlsx
+++ b/XllExamples/Examples.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>Arithmetic Example</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -120,6 +120,9 @@
   <si>
     <t>Divide</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetCircleArea</t>
   </si>
 </sst>
 </file>
@@ -127,20 +130,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -187,7 +190,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -473,26 +476,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H25"/>
+  <dimension ref="B2:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="2.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="4" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:8">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:8">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -511,7 +512,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:8">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -533,7 +534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:8">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -557,7 +558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:8">
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
@@ -581,7 +582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:8">
       <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
@@ -605,76 +606,74 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B9" s="1" t="s">
+    <row r="8" spans="2:8">
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2">
+        <f ca="1">_xll.GetCircleArea(C8)</f>
+        <v>50.265481600000001</v>
+      </c>
+      <c r="G8" s="2">
+        <f>3.1415926*C8*C8</f>
+        <v>50.265481600000001</v>
+      </c>
+      <c r="H8" s="2" t="b">
+        <f ca="1">F8=G8</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B10" s="1" t="s">
+    <row r="11" spans="2:8">
+      <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2" t="s">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B11" s="1" t="s">
+    <row r="12" spans="2:8">
+      <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2" t="str">
-        <f>_xll.ReverseString(C11)</f>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2" t="str">
+        <f>_xll.ReverseString(C12)</f>
         <v>cba</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="2" t="b">
-        <f>F11=G11</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="2">
-        <v>255</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2">
-        <f ca="1">_xll.MultiByteStrLen(REPT(C12,D12))</f>
-        <v>255</v>
-      </c>
-      <c r="G12" s="2">
-        <f>LEN(C12)*D12</f>
-        <v>255</v>
-      </c>
       <c r="H12" s="2" t="b">
-        <f ca="1">F12=G12</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.15">
+        <f>F12=G12</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
       <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
@@ -682,188 +681,189 @@
         <v>16</v>
       </c>
       <c r="D13" s="2">
-        <v>500</v>
+        <v>255</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2">
         <f ca="1">_xll.MultiByteStrLen(REPT(C13,D13))</f>
-        <v>500</v>
+        <v>255</v>
       </c>
       <c r="G13" s="2">
         <f>LEN(C13)*D13</f>
-        <v>500</v>
+        <v>255</v>
       </c>
       <c r="H13" s="2" t="b">
         <f ca="1">F13=G13</f>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B15" s="1" t="s">
+    <row r="14" spans="2:8">
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="2">
+        <v>500</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2">
+        <f ca="1">_xll.MultiByteStrLen(REPT(C14,D14))</f>
+        <v>500</v>
+      </c>
+      <c r="G14" s="2">
+        <f>LEN(C14)*D14</f>
+        <v>500</v>
+      </c>
+      <c r="H14" s="2" t="b">
+        <f ca="1">F14=G14</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B16" s="1" t="s">
+    <row r="17" spans="2:8">
+      <c r="B17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="2" t="s">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B17" s="1" t="s">
+    <row r="18" spans="2:8">
+      <c r="B18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="2">
-        <f t="shared" ref="C17:E19" ca="1" si="0">RANDBETWEEN(1,10)</f>
-        <v>9</v>
-      </c>
-      <c r="D17" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E17" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F17" s="2">
-        <f ca="1">_xll.Trace(C17:E19)</f>
-        <v>20</v>
-      </c>
-      <c r="G17" s="2">
-        <f ca="1">C17+D18+E19</f>
-        <v>20</v>
-      </c>
-      <c r="H17" s="2" t="b">
-        <f ca="1">F17=G17</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.15">
       <c r="C18" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <f t="shared" ref="C18:E20" ca="1" si="0">RANDBETWEEN(1,10)</f>
+        <v>7</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.15">
+        <v>10</v>
+      </c>
+      <c r="F18" s="2">
+        <f ca="1">_xll.Trace(C18:E20)</f>
+        <v>14</v>
+      </c>
+      <c r="G18" s="2">
+        <f ca="1">C18+D19+E20</f>
+        <v>14</v>
+      </c>
+      <c r="H18" s="2" t="b">
+        <f ca="1">F18=G18</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
       <c r="C19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="1" t="s">
+    <row r="20" spans="2:8">
+      <c r="C20" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="1" t="s">
+    <row r="23" spans="2:8">
+      <c r="B23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="2" t="s">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2" t="str">
-        <f ca="1">_xll.VariantType(C23)</f>
-        <v>string</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H23" s="2" t="b">
-        <f ca="1">F23=G23</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:8">
       <c r="B24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="2">
-        <v>100</v>
+      <c r="C24" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="str">
         <f ca="1">_xll.VariantType(C24)</f>
-        <v>double</v>
+        <v>string</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H24" s="2" t="b">
         <f ca="1">F24=G24</f>
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:8">
       <c r="B25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="4">
-        <v>40179</v>
-      </c>
-      <c r="D25" s="5">
-        <f>C25</f>
-        <v>40179</v>
-      </c>
+      <c r="C25" s="2">
+        <v>100</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
       <c r="F25" s="2" t="str">
-        <f ca="1">_xll.VariantType(C25,D25)</f>
+        <f ca="1">_xll.VariantType(C25)</f>
         <v>double</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -871,6 +871,29 @@
       </c>
       <c r="H25" s="2" t="b">
         <f ca="1">F25=G25</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="4">
+        <v>40179</v>
+      </c>
+      <c r="D26" s="5">
+        <f>C26</f>
+        <v>40179</v>
+      </c>
+      <c r="F26" s="2" t="str">
+        <f ca="1">_xll.VariantType(C26,D26)</f>
+        <v>double</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="2" t="b">
+        <f ca="1">F26=G26</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>